<commit_message>
updated perimeter in Annie config inputs
</commit_message>
<xml_diff>
--- a/AnnieLake/ConfigurationInputsAnnie.xlsx
+++ b/AnnieLake/ConfigurationInputsAnnie.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Ian_GIS\gleon\SOS\AnnieLake\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="60" windowWidth="8595" windowHeight="7740"/>
   </bookViews>
@@ -140,8 +135,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,7 +241,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -278,10 +273,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -313,7 +307,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -489,20 +482,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,23 +506,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2334.768</v>
+        <v>3062</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -540,7 +533,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -551,7 +544,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -562,7 +555,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -573,7 +566,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -584,12 +577,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -600,12 +593,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -616,7 +609,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -627,7 +620,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -638,7 +631,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -649,7 +642,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -660,7 +653,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -671,7 +664,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -682,12 +675,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -698,7 +691,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -709,7 +702,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -720,12 +713,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -743,24 +736,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
edited Annie TS to include volume & sw_doc. Added ProdStartDay& ProdEndDay to config file
</commit_message>
<xml_diff>
--- a/AnnieLake/ConfigurationInputsAnnie.xlsx
+++ b/AnnieLake/ConfigurationInputsAnnie.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>Parameter</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>DOC_gw = InLakeDOC</t>
+  </si>
+  <si>
+    <t>ProdStartDay</t>
+  </si>
+  <si>
+    <t>ProdEndDay</t>
   </si>
 </sst>
 </file>
@@ -483,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -727,6 +733,22 @@
       </c>
       <c r="C26" s="6" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="7">
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dynamic GW/SW change for Lake Annie.
</commit_message>
<xml_diff>
--- a/AnnieLake/ConfigurationInputsAnnie.xlsx
+++ b/AnnieLake/ConfigurationInputsAnnie.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="60" windowWidth="8595" windowHeight="7740"/>
@@ -141,8 +141,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +279,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -313,6 +314,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -488,20 +490,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,12 +514,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -528,7 +530,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -539,7 +541,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75">
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -550,7 +552,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75">
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -561,7 +563,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -572,7 +574,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -583,12 +585,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -599,12 +601,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -615,7 +617,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -626,7 +628,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -637,7 +639,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -648,7 +650,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -659,7 +661,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -670,7 +672,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -681,12 +683,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -697,7 +699,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -708,7 +710,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -719,12 +721,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -735,20 +737,20 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B28" s="7">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -758,24 +760,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>